<commit_message>
before changing regressions to not include multiple lawyer types in predictor variables
</commit_message>
<xml_diff>
--- a/Administrative-Noam/LoggedHours.xlsx
+++ b/Administrative-Noam/LoggedHours.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17960" yWindow="460" windowWidth="13080" windowHeight="12220" tabRatio="500"/>
+    <workbookView xWindow="14360" yWindow="460" windowWidth="11760" windowHeight="12220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="103">
   <si>
     <t>Date</t>
   </si>
@@ -324,6 +324,18 @@
   </si>
   <si>
     <t>Monday, Jan 22, 2018</t>
+  </si>
+  <si>
+    <t>Thursday, Jan 25, 2018</t>
+  </si>
+  <si>
+    <t>Friday, Jan 26, 2018</t>
+  </si>
+  <si>
+    <t>BiWeek of 2/1/18-2/15/18</t>
+  </si>
+  <si>
+    <t>Thursday, Feb 1, 2018</t>
   </si>
 </sst>
 </file>
@@ -348,12 +360,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Helvetica"/>
     </font>
     <font>
       <sz val="12"/>
@@ -383,6 +389,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -401,46 +413,55 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -450,6 +471,7 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -459,6 +481,7 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -734,38 +757,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E282"/>
+  <dimension ref="A1:E302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A266" zoomScale="98" workbookViewId="0">
-      <selection activeCell="D276" sqref="D276"/>
+    <sheetView tabSelected="1" topLeftCell="A282" zoomScale="98" workbookViewId="0">
+      <selection activeCell="D289" sqref="D289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" customWidth="1"/>
-    <col min="2" max="3" width="10.83203125" style="2"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" style="9" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="10"/>
+    <col min="4" max="4" width="12.33203125" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -773,13 +797,13 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="10">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="10">
         <v>0.70833333333333337</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="11">
         <f>C4-B4</f>
         <v>4.1666666666666741E-2</v>
       </c>
@@ -788,13 +812,13 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="10">
         <v>6.25E-2</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="10">
         <v>0.14583333333333334</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="11">
         <f t="shared" ref="D5:D17" si="0">C5-B5</f>
         <v>8.3333333333333343E-2</v>
       </c>
@@ -803,13 +827,13 @@
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="10">
         <v>0.625</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="10">
         <v>0.64583333333333337</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="11">
         <f t="shared" si="0"/>
         <v>2.083333333333337E-2</v>
       </c>
@@ -818,13 +842,13 @@
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="10">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="10">
         <v>0.72916666666666663</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="11">
         <f t="shared" si="0"/>
         <v>0.14583333333333326</v>
       </c>
@@ -833,13 +857,13 @@
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="10">
         <v>0.75</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="10">
         <v>0.79166666666666663</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="11">
         <f t="shared" si="0"/>
         <v>4.166666666666663E-2</v>
       </c>
@@ -848,13 +872,13 @@
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="10">
         <v>0.64583333333333337</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="10">
         <v>0.6875</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="11">
         <f t="shared" si="0"/>
         <v>4.166666666666663E-2</v>
       </c>
@@ -863,13 +887,13 @@
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="10">
         <v>0.82291666666666663</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="10">
         <v>0.97916666666666663</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="11">
         <f t="shared" si="0"/>
         <v>0.15625</v>
       </c>
@@ -878,13 +902,13 @@
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="10">
         <v>0.53125</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="10">
         <v>0.5625</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="11">
         <f t="shared" si="0"/>
         <v>3.125E-2</v>
       </c>
@@ -893,13 +917,13 @@
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="10">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="10">
         <v>0.61458333333333337</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="11">
         <f t="shared" si="0"/>
         <v>3.125E-2</v>
       </c>
@@ -908,13 +932,13 @@
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="10">
         <v>0.13541666666666666</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="10">
         <v>0.17708333333333334</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="11">
         <f t="shared" si="0"/>
         <v>4.1666666666666685E-2</v>
       </c>
@@ -923,13 +947,13 @@
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="10">
         <v>0.375</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="10">
         <v>0.40625</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="11">
         <f t="shared" si="0"/>
         <v>3.125E-2</v>
       </c>
@@ -938,13 +962,13 @@
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="10">
         <v>0.65625</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="10">
         <v>0.71875</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="11">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
@@ -953,13 +977,13 @@
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="10">
         <v>0.82291666666666663</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="10">
         <v>0.88541666666666663</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="11">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
@@ -968,48 +992,48 @@
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="10">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="10">
         <v>0.625</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="11">
         <f t="shared" si="0"/>
         <v>4.166666666666663E-2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="11">
         <f>SUM(D4:D17)</f>
         <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="D19" s="11"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="5" t="s">
+      <c r="A22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1017,13 +1041,13 @@
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="10">
         <v>0.84722222222222221</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="10">
         <v>0.91666666666666663</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="11">
         <f>C23-B23</f>
         <v>6.944444444444442E-2</v>
       </c>
@@ -1032,13 +1056,13 @@
       <c r="A24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="10">
         <v>0.375</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="10">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="11">
         <f t="shared" ref="D24:D36" si="1">C24-B24</f>
         <v>4.1666666666666685E-2</v>
       </c>
@@ -1047,13 +1071,13 @@
       <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="10">
         <v>0.5625</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="10">
         <v>0.59375</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="11">
         <f t="shared" si="1"/>
         <v>3.125E-2</v>
       </c>
@@ -1062,13 +1086,13 @@
       <c r="A26" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="10">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="10">
         <v>0.72916666666666663</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="11">
         <f t="shared" si="1"/>
         <v>6.25E-2</v>
       </c>
@@ -1077,13 +1101,13 @@
       <c r="A27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="10">
         <v>0.88541666666666663</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="10">
         <v>0.9375</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="11">
         <f t="shared" si="1"/>
         <v>5.208333333333337E-2</v>
       </c>
@@ -1092,13 +1116,13 @@
       <c r="A28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="10">
         <v>0.51041666666666663</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="10">
         <v>0.56944444444444442</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="11">
         <f t="shared" si="1"/>
         <v>5.902777777777779E-2</v>
       </c>
@@ -1107,2035 +1131,2035 @@
       <c r="A29" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="10">
         <v>0.375</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="10">
         <v>0.4375</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="11">
         <f t="shared" si="1"/>
         <v>6.25E-2</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
-      <c r="D30" s="3">
+      <c r="D30" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
-      <c r="D31" s="3">
+      <c r="D31" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
-      <c r="D32" s="3">
+      <c r="D32" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
-      <c r="D33" s="3">
+      <c r="D33" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
-      <c r="D34" s="3">
+      <c r="D34" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
-      <c r="D35" s="3">
+      <c r="D35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
-      <c r="D36" s="3">
+      <c r="D36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="11">
         <f>SUM(D23:D36)</f>
         <v>0.37847222222222227</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41" s="5" t="s">
+      <c r="A41" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="A42" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="10">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="10">
         <v>0.625</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="11">
         <f>C42-B42</f>
         <v>4.166666666666663E-2</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="A43" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="10">
         <v>0.5625</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="10">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="11">
         <f t="shared" ref="D43:D53" si="2">C43-B43</f>
         <v>0.10416666666666663</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="A44" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="10">
         <v>0.59722222222222221</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="10">
         <v>0.67708333333333337</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="11">
         <f t="shared" si="2"/>
         <v>7.986111111111116E-2</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="A45" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="10">
         <v>0.5</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="10">
         <v>0.625</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="11">
         <f t="shared" si="2"/>
         <v>0.125</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="A46" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46" s="10">
         <v>0.55208333333333337</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="10">
         <v>0.61805555555555558</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="11">
         <f t="shared" si="2"/>
         <v>6.597222222222221E-2</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="A47" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="10">
         <v>0.8125</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="10">
         <v>0.91666666666666663</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="11">
         <f t="shared" si="2"/>
         <v>0.10416666666666663</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="A48" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="10">
         <v>0.61805555555555558</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="10">
         <v>0.65972222222222221</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="11">
         <f t="shared" si="2"/>
         <v>4.166666666666663E-2</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="A49" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="10">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="10">
         <v>0.77083333333333337</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D49" s="11">
         <f t="shared" si="2"/>
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D50" s="3">
+      <c r="D50" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D51" s="3">
+      <c r="D51" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D52" s="3">
+      <c r="D52" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D53" s="3">
+      <c r="D53" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D54" s="11">
         <f>SUM(D42:D53)</f>
         <v>0.62499999999999989</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D55" s="3"/>
-    </row>
-    <row r="57" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
+      <c r="D55" s="11"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B57" s="9"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B59" s="5" t="s">
+      <c r="A59" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C59" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="A60" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B60" s="10">
         <v>0.875</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60" s="10">
         <v>0.91666666666666663</v>
       </c>
-      <c r="D60" s="3">
+      <c r="D60" s="11">
         <f>C60-B60</f>
         <v>4.166666666666663E-2</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+      <c r="A61" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B61" s="10">
         <v>0.83333333333333337</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61" s="10">
         <v>0.875</v>
       </c>
-      <c r="D61" s="3">
+      <c r="D61" s="11">
         <f t="shared" ref="D61:D71" si="3">C61-B61</f>
         <v>4.166666666666663E-2</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="A62" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62" s="10">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="10">
         <v>6.25E-2</v>
       </c>
-      <c r="D62" s="3">
+      <c r="D62" s="11">
         <f t="shared" si="3"/>
         <v>4.1666666666666671E-2</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+      <c r="A63" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63" s="10">
         <v>0.89583333333333337</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63" s="10">
         <v>0.97916666666666663</v>
       </c>
-      <c r="D63" s="3">
+      <c r="D63" s="11">
         <f t="shared" si="3"/>
         <v>8.3333333333333259E-2</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+      <c r="A64" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64" s="10">
         <v>0.91666666666666663</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64" s="10">
         <v>0.99652777777777779</v>
       </c>
-      <c r="D64" s="3">
+      <c r="D64" s="11">
         <f t="shared" si="3"/>
         <v>7.986111111111116E-2</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+      <c r="A65" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B65" s="10">
         <v>0.90625</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C65" s="10">
         <v>0.97916666666666663</v>
       </c>
-      <c r="D65" s="3">
+      <c r="D65" s="11">
         <f t="shared" si="3"/>
         <v>7.291666666666663E-2</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+      <c r="A66" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B66" s="10">
         <v>0.3125</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C66" s="10">
         <v>0.35416666666666669</v>
       </c>
-      <c r="D66" s="3">
+      <c r="D66" s="11">
         <f>C66-B66</f>
         <v>4.1666666666666685E-2</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D67" s="3">
+      <c r="D67" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D68" s="3">
+      <c r="D68" s="11">
         <f>C68-B68</f>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D69" s="3">
+      <c r="D69" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D70" s="3">
+      <c r="D70" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D71" s="3">
+      <c r="D71" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C72" s="2" t="s">
+      <c r="C72" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D72" s="3">
+      <c r="D72" s="11">
         <f>SUM(D60:D71)</f>
         <v>0.40277777777777768</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A75" s="9" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B75" s="9"/>
-      <c r="C75" s="9"/>
-      <c r="D75" s="9"/>
+      <c r="B75" s="12"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B77" s="5" t="s">
+      <c r="A77" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C77" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D77" s="4" t="s">
+      <c r="D77" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+      <c r="A78" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B78" s="2">
+      <c r="B78" s="10">
         <v>0.875</v>
       </c>
-      <c r="C78" s="2">
+      <c r="C78" s="10">
         <v>0.95833333333333337</v>
       </c>
-      <c r="D78" s="3">
+      <c r="D78" s="11">
         <f>C78-B78</f>
         <v>8.333333333333337E-2</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+      <c r="A79" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B79" s="10">
         <v>0.75</v>
       </c>
-      <c r="C79" s="2">
+      <c r="C79" s="10">
         <v>0.79166666666666663</v>
       </c>
-      <c r="D79" s="3">
+      <c r="D79" s="11">
         <f t="shared" ref="D79:D83" si="4">C79-B79</f>
         <v>4.166666666666663E-2</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+      <c r="A80" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B80" s="10">
         <v>0.86111111111111116</v>
       </c>
-      <c r="C80" s="2">
+      <c r="C80" s="10">
         <v>0.90277777777777779</v>
       </c>
-      <c r="D80" s="3">
+      <c r="D80" s="11">
         <f t="shared" si="4"/>
         <v>4.166666666666663E-2</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+      <c r="A81" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B81" s="2">
+      <c r="B81" s="10">
         <v>0.9375</v>
       </c>
-      <c r="C81" s="2">
+      <c r="C81" s="10">
         <v>0.97916666666666663</v>
       </c>
-      <c r="D81" s="3">
+      <c r="D81" s="11">
         <f t="shared" si="4"/>
         <v>4.166666666666663E-2</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D82" s="3">
+      <c r="D82" s="11">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D83" s="3">
+      <c r="D83" s="11">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D84" s="3">
+      <c r="D84" s="11">
         <f>C84-B84</f>
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D85" s="3">
+      <c r="D85" s="11">
         <f t="shared" ref="D85" si="5">C85-B85</f>
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D86" s="3">
+      <c r="D86" s="11">
         <f>C86-B86</f>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D87" s="3">
+      <c r="D87" s="11">
         <f t="shared" ref="D87:D89" si="6">C87-B87</f>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D88" s="3">
+      <c r="D88" s="11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D89" s="3">
+      <c r="D89" s="11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C90" s="2" t="s">
+      <c r="C90" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D90" s="3">
+      <c r="D90" s="11">
         <f>SUM(D78:D89)</f>
         <v>0.20833333333333326</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A93" s="9" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B93" s="9"/>
-      <c r="C93" s="9"/>
-      <c r="D93" s="9"/>
+      <c r="B93" s="12"/>
+      <c r="C93" s="12"/>
+      <c r="D93" s="12"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B95" s="5" t="s">
+      <c r="A95" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B95" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C95" s="5" t="s">
+      <c r="C95" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D95" s="4" t="s">
+      <c r="D95" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
+      <c r="A96" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B96" s="2">
-        <v>0</v>
-      </c>
-      <c r="C96" s="2">
+      <c r="B96" s="10">
+        <v>0</v>
+      </c>
+      <c r="C96" s="10">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D96" s="3">
+      <c r="D96" s="11">
         <f>C96-B96</f>
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
+      <c r="A97" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B97" s="2">
+      <c r="B97" s="10">
         <v>0.79166666666666663</v>
       </c>
-      <c r="C97" s="2">
+      <c r="C97" s="10">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D97" s="3">
+      <c r="D97" s="11">
         <f t="shared" ref="D97:D99" si="7">C97-B97</f>
         <v>4.1666666666666741E-2</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
+      <c r="A98" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B98" s="2">
+      <c r="B98" s="10">
         <v>0.89513888888888893</v>
       </c>
-      <c r="C98" s="2">
+      <c r="C98" s="10">
         <v>0.99930555555555556</v>
       </c>
-      <c r="D98" s="3">
+      <c r="D98" s="11">
         <f t="shared" si="7"/>
         <v>0.10416666666666663</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
+      <c r="A99" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B99" s="2">
-        <v>0</v>
-      </c>
-      <c r="C99" s="2">
+      <c r="B99" s="10">
+        <v>0</v>
+      </c>
+      <c r="C99" s="10">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D99" s="3">
+      <c r="D99" s="11">
         <f t="shared" si="7"/>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
+      <c r="A100" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B100" s="2">
+      <c r="B100" s="10">
         <v>0.85416666666666663</v>
       </c>
-      <c r="C100" s="2">
+      <c r="C100" s="10">
         <v>0.90625</v>
       </c>
-      <c r="D100" s="3">
+      <c r="D100" s="11">
         <f>C100-B100</f>
         <v>5.208333333333337E-2</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
+      <c r="A101" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B101" s="2">
+      <c r="B101" s="10">
         <v>0.8125</v>
       </c>
-      <c r="C101" s="2">
+      <c r="C101" s="10">
         <v>0.875</v>
       </c>
-      <c r="D101" s="3">
+      <c r="D101" s="11">
         <f>C101-B101</f>
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D102" s="3">
+      <c r="D102" s="11">
         <f>C102-B102</f>
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D103" s="3">
+      <c r="D103" s="11">
         <f t="shared" ref="D103" si="8">C103-B103</f>
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D104" s="3">
+      <c r="D104" s="11">
         <f>C104-B104</f>
         <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D105" s="3">
+      <c r="D105" s="11">
         <f t="shared" ref="D105:D107" si="9">C105-B105</f>
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D106" s="3">
+      <c r="D106" s="11">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D107" s="3">
+      <c r="D107" s="11">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C108" s="2" t="s">
+      <c r="C108" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D108" s="3">
+      <c r="D108" s="11">
         <f>SUM(D96:D107)</f>
         <v>0.38541666666666674</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A110" s="9" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B110" s="9"/>
-      <c r="C110" s="9"/>
-      <c r="D110" s="9"/>
+      <c r="B110" s="12"/>
+      <c r="C110" s="12"/>
+      <c r="D110" s="12"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A112" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B112" s="5" t="s">
+      <c r="A112" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B112" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C112" s="5" t="s">
+      <c r="C112" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D112" s="4" t="s">
+      <c r="D112" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
+      <c r="A113" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B113" s="2">
+      <c r="B113" s="10">
         <v>0.90625</v>
       </c>
-      <c r="C113" s="2">
+      <c r="C113" s="10">
         <v>0.94791666666666663</v>
       </c>
-      <c r="D113" s="3">
+      <c r="D113" s="11">
         <f>C113-B113</f>
         <v>4.166666666666663E-2</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
+      <c r="A114" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B114" s="2">
+      <c r="B114" s="10">
         <v>0.83333333333333337</v>
       </c>
-      <c r="C114" s="2">
+      <c r="C114" s="10">
         <v>0.85416666666666663</v>
       </c>
-      <c r="D114" s="3">
+      <c r="D114" s="11">
         <f t="shared" ref="D114:D116" si="10">C114-B114</f>
         <v>2.0833333333333259E-2</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
+      <c r="A115" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B115" s="2">
+      <c r="B115" s="10">
         <v>0.6875</v>
       </c>
-      <c r="C115" s="2">
+      <c r="C115" s="10">
         <v>0.77083333333333337</v>
       </c>
-      <c r="D115" s="3">
+      <c r="D115" s="11">
         <f t="shared" si="10"/>
         <v>8.333333333333337E-2</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
+      <c r="A116" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B116" s="2">
+      <c r="B116" s="10">
         <v>0.82291666666666663</v>
       </c>
-      <c r="C116" s="2">
+      <c r="C116" s="10">
         <v>0.91666666666666663</v>
       </c>
-      <c r="D116" s="3">
+      <c r="D116" s="11">
         <f t="shared" si="10"/>
         <v>9.375E-2</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
+      <c r="A117" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B117" s="2">
+      <c r="B117" s="10">
         <v>0.84722222222222221</v>
       </c>
-      <c r="C117" s="2">
+      <c r="C117" s="10">
         <v>0.86805555555555547</v>
       </c>
-      <c r="D117" s="3">
+      <c r="D117" s="11">
         <f>C117-B117</f>
         <v>2.0833333333333259E-2</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D118" s="3">
+      <c r="D118" s="11">
         <f>C118-B118</f>
         <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D119" s="3">
+      <c r="D119" s="11">
         <f>C119-B119</f>
         <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D120" s="3">
+      <c r="D120" s="11">
         <f t="shared" ref="D120" si="11">C120-B120</f>
         <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D121" s="3">
+      <c r="D121" s="11">
         <f>C121-B121</f>
         <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D122" s="3">
+      <c r="D122" s="11">
         <f t="shared" ref="D122:D124" si="12">C122-B122</f>
         <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D123" s="3">
+      <c r="D123" s="11">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D124" s="3">
+      <c r="D124" s="11">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C125" s="2" t="s">
+      <c r="C125" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D125" s="3">
+      <c r="D125" s="11">
         <f>SUM(D113:D124)</f>
         <v>0.26041666666666652</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A127" s="9" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B127" s="9"/>
-      <c r="C127" s="9"/>
-      <c r="D127" s="9"/>
+      <c r="B127" s="12"/>
+      <c r="C127" s="12"/>
+      <c r="D127" s="12"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A129" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B129" s="5" t="s">
+      <c r="A129" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B129" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C129" s="5" t="s">
+      <c r="C129" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D129" s="4" t="s">
+      <c r="D129" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
+      <c r="A130" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B130" s="2">
+      <c r="B130" s="10">
         <v>0.625</v>
       </c>
-      <c r="C130" s="2">
+      <c r="C130" s="10">
         <v>0.69791666666666663</v>
       </c>
-      <c r="D130" s="3">
+      <c r="D130" s="11">
         <f>C130-B130</f>
         <v>7.291666666666663E-2</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
+      <c r="A131" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B131" s="2">
-        <v>0</v>
-      </c>
-      <c r="C131" s="2">
+      <c r="B131" s="10">
+        <v>0</v>
+      </c>
+      <c r="C131" s="10">
         <v>5.2083333333333336E-2</v>
       </c>
-      <c r="D131" s="3">
+      <c r="D131" s="11">
         <f t="shared" ref="D131:D133" si="13">C131-B131</f>
         <v>5.2083333333333336E-2</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
+      <c r="A132" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B132" s="2">
+      <c r="B132" s="10">
         <v>0.35416666666666669</v>
       </c>
-      <c r="C132" s="2">
+      <c r="C132" s="10">
         <v>0.38541666666666669</v>
       </c>
-      <c r="D132" s="3">
+      <c r="D132" s="11">
         <f t="shared" si="13"/>
         <v>3.125E-2</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D133" s="3">
+      <c r="D133" s="11">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D134" s="3">
+      <c r="D134" s="11">
         <f>C134-B134</f>
         <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D135" s="3">
+      <c r="D135" s="11">
         <f>C135-B135</f>
         <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D136" s="3">
+      <c r="D136" s="11">
         <f>C136-B136</f>
         <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D137" s="3">
+      <c r="D137" s="11">
         <f t="shared" ref="D137" si="14">C137-B137</f>
         <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D138" s="3">
+      <c r="D138" s="11">
         <f>C138-B138</f>
         <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D139" s="3">
+      <c r="D139" s="11">
         <f t="shared" ref="D139:D141" si="15">C139-B139</f>
         <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D140" s="3">
+      <c r="D140" s="11">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D141" s="3">
+      <c r="D141" s="11">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C142" s="2" t="s">
+      <c r="C142" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D142" s="3">
+      <c r="D142" s="11">
         <f>SUM(D130:D141)</f>
         <v>0.15624999999999997</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A145" s="9" t="s">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B145" s="9"/>
-      <c r="C145" s="9"/>
-      <c r="D145" s="9"/>
+      <c r="B145" s="12"/>
+      <c r="C145" s="12"/>
+      <c r="D145" s="12"/>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A147" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B147" s="5" t="s">
+      <c r="A147" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B147" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C147" s="5" t="s">
+      <c r="C147" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D147" s="4" t="s">
+      <c r="D147" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
+      <c r="A148" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B148" s="2">
+      <c r="B148" s="10">
         <v>0.39583333333333331</v>
       </c>
-      <c r="C148" s="2">
+      <c r="C148" s="10">
         <v>0.44791666666666669</v>
       </c>
-      <c r="D148" s="3">
+      <c r="D148" s="11">
         <f>C148-B148</f>
         <v>5.208333333333337E-2</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
+      <c r="A149" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B149" s="2">
+      <c r="B149" s="10">
         <v>0.89583333333333337</v>
       </c>
-      <c r="C149" s="2">
+      <c r="C149" s="10">
         <v>0.91666666666666663</v>
       </c>
-      <c r="D149" s="3">
+      <c r="D149" s="11">
         <f>C149-B149</f>
         <v>2.0833333333333259E-2</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
+      <c r="A150" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B150" s="2">
+      <c r="B150" s="10">
         <v>0.4375</v>
       </c>
-      <c r="C150" s="2">
+      <c r="C150" s="10">
         <v>0.5</v>
       </c>
-      <c r="D150" s="3">
+      <c r="D150" s="11">
         <f t="shared" ref="D150" si="16">C150-B150</f>
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A151" s="6" t="s">
+      <c r="A151" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B151" s="2">
+      <c r="B151" s="10">
         <v>0.54166666666666663</v>
       </c>
-      <c r="C151" s="2">
+      <c r="C151" s="10">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D151" s="3">
+      <c r="D151" s="11">
         <f>C151-B151</f>
         <v>4.1666666666666741E-2</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
+      <c r="A152" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B152" s="2">
+      <c r="B152" s="10">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C152" s="2">
+      <c r="C152" s="10">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D152" s="3">
+      <c r="D152" s="11">
         <f>C152-B152</f>
         <v>0.10416666666666669</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D153" s="3">
+      <c r="D153" s="11">
         <f>C153-B153</f>
         <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D154" s="3">
+      <c r="D154" s="11">
         <f>C154-B154</f>
         <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D155" s="3">
+      <c r="D155" s="11">
         <f t="shared" ref="D155" si="17">C155-B155</f>
         <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D156" s="3">
+      <c r="D156" s="11">
         <f>C156-B156</f>
         <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D157" s="3">
+      <c r="D157" s="11">
         <f t="shared" ref="D157:D159" si="18">C157-B157</f>
         <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D158" s="3">
+      <c r="D158" s="11">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D159" s="3">
+      <c r="D159" s="11">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C160" s="2" t="s">
+      <c r="C160" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D160" s="3">
+      <c r="D160" s="11">
         <f>SUM(D148:D159)</f>
         <v>0.28125000000000006</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A162" s="9" t="s">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B162" s="9"/>
-      <c r="C162" s="9"/>
-      <c r="D162" s="9"/>
+      <c r="B162" s="12"/>
+      <c r="C162" s="12"/>
+      <c r="D162" s="12"/>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A164" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B164" s="5" t="s">
+      <c r="A164" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B164" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C164" s="5" t="s">
+      <c r="C164" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D164" s="4" t="s">
+      <c r="D164" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A165" t="s">
+      <c r="A165" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B165" s="2">
+      <c r="B165" s="10">
         <v>0.6875</v>
       </c>
-      <c r="C165" s="2">
+      <c r="C165" s="10">
         <v>0.70833333333333337</v>
       </c>
-      <c r="D165" s="3">
+      <c r="D165" s="11">
         <f>C165-B165</f>
         <v>2.083333333333337E-2</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A166" t="s">
+      <c r="A166" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B166" s="2">
+      <c r="B166" s="10">
         <v>0.6875</v>
       </c>
-      <c r="C166" s="2">
+      <c r="C166" s="10">
         <v>0.70833333333333337</v>
       </c>
-      <c r="D166" s="3">
+      <c r="D166" s="11">
         <f>C166-B166</f>
         <v>2.083333333333337E-2</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
+      <c r="A167" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B167" s="2">
+      <c r="B167" s="10">
         <v>0.83263888888888893</v>
       </c>
-      <c r="C167" s="2">
+      <c r="C167" s="10">
         <v>0.99930555555555556</v>
       </c>
-      <c r="D167" s="3">
+      <c r="D167" s="11">
         <f t="shared" ref="D167" si="19">C167-B167</f>
         <v>0.16666666666666663</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A168" s="6" t="s">
+      <c r="A168" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B168" s="2">
-        <v>0</v>
-      </c>
-      <c r="C168" s="2">
+      <c r="B168" s="10">
+        <v>0</v>
+      </c>
+      <c r="C168" s="10">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D168" s="3">
+      <c r="D168" s="11">
         <f>C168-B168</f>
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A169" t="s">
+      <c r="A169" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B169" s="2">
+      <c r="B169" s="10">
         <v>0.39583333333333331</v>
       </c>
-      <c r="C169" s="2">
+      <c r="C169" s="10">
         <v>0.4375</v>
       </c>
-      <c r="D169" s="3">
+      <c r="D169" s="11">
         <f>C169-B169</f>
         <v>4.1666666666666685E-2</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A170" t="s">
+      <c r="A170" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B170" s="2">
+      <c r="B170" s="10">
         <v>0.64583333333333337</v>
       </c>
-      <c r="C170" s="2">
+      <c r="C170" s="10">
         <v>0.6875</v>
       </c>
-      <c r="D170" s="3">
+      <c r="D170" s="11">
         <f>C170-B170</f>
         <v>4.166666666666663E-2</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A171" t="s">
+      <c r="A171" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B171" s="2">
+      <c r="B171" s="10">
         <v>0.63541666666666663</v>
       </c>
-      <c r="C171" s="2">
+      <c r="C171" s="10">
         <v>0.67708333333333337</v>
       </c>
-      <c r="D171" s="3">
+      <c r="D171" s="11">
         <f>C171-B171</f>
         <v>4.1666666666666741E-2</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A172" t="s">
+      <c r="A172" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B172" s="2">
+      <c r="B172" s="10">
         <v>0.57638888888888895</v>
       </c>
-      <c r="C172" s="2">
+      <c r="C172" s="10">
         <v>0.63888888888888895</v>
       </c>
-      <c r="D172" s="3">
+      <c r="D172" s="11">
         <f t="shared" ref="D172" si="20">C172-B172</f>
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A173" t="s">
+      <c r="A173" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B173" s="2">
+      <c r="B173" s="10">
         <v>0.4375</v>
       </c>
-      <c r="C173" s="2">
+      <c r="C173" s="10">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D173" s="3">
+      <c r="D173" s="11">
         <f>C173-B173</f>
         <v>0.10416666666666663</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D174" s="3">
+      <c r="D174" s="11">
         <f t="shared" ref="D174:D176" si="21">C174-B174</f>
         <v>0</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D175" s="3">
+      <c r="D175" s="11">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D176" s="3">
+      <c r="D176" s="11">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C177" s="2" t="s">
+      <c r="C177" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D177" s="3">
+      <c r="D177" s="11">
         <f>SUM(D165:D176)</f>
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A180" s="9" t="s">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A180" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B180" s="9"/>
-      <c r="C180" s="9"/>
-      <c r="D180" s="9"/>
+      <c r="B180" s="12"/>
+      <c r="C180" s="12"/>
+      <c r="D180" s="12"/>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A182" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B182" s="5" t="s">
+      <c r="A182" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B182" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C182" s="5" t="s">
+      <c r="C182" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D182" s="4" t="s">
+      <c r="D182" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A183" t="s">
+      <c r="A183" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B183" s="2">
+      <c r="B183" s="10">
         <v>0.89583333333333337</v>
       </c>
-      <c r="C183" s="2">
+      <c r="C183" s="10">
         <v>0.92708333333333337</v>
       </c>
-      <c r="D183" s="3">
+      <c r="D183" s="11">
         <f>C183-B183</f>
         <v>3.125E-2</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A184" t="s">
+      <c r="A184" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B184" s="2">
+      <c r="B184" s="10">
         <v>0.63541666666666663</v>
       </c>
-      <c r="C184" s="2">
+      <c r="C184" s="10">
         <v>0.68055555555555547</v>
       </c>
-      <c r="D184" s="3">
+      <c r="D184" s="11">
         <f>C184-B184</f>
         <v>4.513888888888884E-2</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A185" t="s">
+      <c r="A185" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B185" s="2">
+      <c r="B185" s="10">
         <v>0.625</v>
       </c>
-      <c r="C185" s="2">
+      <c r="C185" s="10">
         <v>0.77083333333333337</v>
       </c>
-      <c r="D185" s="3">
+      <c r="D185" s="11">
         <f t="shared" ref="D185" si="22">C185-B185</f>
         <v>0.14583333333333337</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A186" s="6" t="s">
+      <c r="A186" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B186" s="2">
+      <c r="B186" s="10">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C186" s="2">
+      <c r="C186" s="10">
         <v>0.78125</v>
       </c>
-      <c r="D186" s="3">
+      <c r="D186" s="11">
         <f>C186-B186</f>
         <v>7.291666666666663E-2</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D187" s="3">
+      <c r="D187" s="11">
         <f>C187-B187</f>
         <v>0</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D188" s="3">
+      <c r="D188" s="11">
         <f>C188-B188</f>
         <v>0</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D189" s="3">
+      <c r="D189" s="11">
         <f>C189-B189</f>
         <v>0</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D190" s="3">
+      <c r="D190" s="11">
         <f t="shared" ref="D190" si="23">C190-B190</f>
         <v>0</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D191" s="3">
+      <c r="D191" s="11">
         <f>C191-B191</f>
         <v>0</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D192" s="3">
+      <c r="D192" s="11">
         <f t="shared" ref="D192:D194" si="24">C192-B192</f>
         <v>0</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D193" s="3">
+      <c r="D193" s="11">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D194" s="3">
+      <c r="D194" s="11">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C195" s="2" t="s">
+      <c r="C195" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D195" s="3">
+      <c r="D195" s="11">
         <f>SUM(D183:D194)</f>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A198" s="9" t="s">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A198" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B198" s="9"/>
-      <c r="C198" s="9"/>
-      <c r="D198" s="9"/>
+      <c r="B198" s="12"/>
+      <c r="C198" s="12"/>
+      <c r="D198" s="12"/>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A200" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B200" s="5" t="s">
+      <c r="A200" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B200" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C200" s="5" t="s">
+      <c r="C200" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D200" s="4" t="s">
+      <c r="D200" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A201" t="s">
+      <c r="A201" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B201" s="2">
+      <c r="B201" s="10">
         <v>0.5</v>
       </c>
-      <c r="C201" s="2">
+      <c r="C201" s="10">
         <v>0.55555555555555558</v>
       </c>
-      <c r="D201" s="3">
+      <c r="D201" s="11">
         <f>C201-B201</f>
         <v>5.555555555555558E-2</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A202" t="s">
+      <c r="A202" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B202" s="2">
+      <c r="B202" s="10">
         <v>0.59027777777777779</v>
       </c>
-      <c r="C202" s="2">
+      <c r="C202" s="10">
         <v>0.6875</v>
       </c>
-      <c r="D202" s="3">
+      <c r="D202" s="11">
         <f>C202-B202</f>
         <v>9.722222222222221E-2</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A203" t="s">
+      <c r="A203" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B203" s="2">
+      <c r="B203" s="10">
         <v>0.29166666666666669</v>
       </c>
-      <c r="C203" s="2">
+      <c r="C203" s="10">
         <v>0.35416666666666669</v>
       </c>
-      <c r="D203" s="3">
+      <c r="D203" s="11">
         <f t="shared" ref="D203" si="25">C203-B203</f>
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A204" s="6"/>
-      <c r="D204" s="3">
+      <c r="A204" s="4"/>
+      <c r="D204" s="11">
         <f>C204-B204</f>
         <v>0</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D205" s="3">
+      <c r="D205" s="11">
         <f>C205-B205</f>
         <v>0</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D206" s="3">
+      <c r="D206" s="11">
         <f>C206-B206</f>
         <v>0</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D207" s="3">
+      <c r="D207" s="11">
         <f>C207-B207</f>
         <v>0</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D208" s="3">
+      <c r="D208" s="11">
         <f t="shared" ref="D208" si="26">C208-B208</f>
         <v>0</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D209" s="3">
+      <c r="D209" s="11">
         <f>C209-B209</f>
         <v>0</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D210" s="3">
+      <c r="D210" s="11">
         <f t="shared" ref="D210:D212" si="27">C210-B210</f>
         <v>0</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D211" s="3">
+      <c r="D211" s="11">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D212" s="3">
+      <c r="D212" s="11">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C213" s="2" t="s">
+      <c r="C213" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D213" s="3">
+      <c r="D213" s="11">
         <f>SUM(D201:D212)</f>
         <v>0.21527777777777779</v>
       </c>
     </row>
-    <row r="215" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A215" s="9" t="s">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A215" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B215" s="9"/>
-      <c r="C215" s="9"/>
-      <c r="D215" s="9"/>
+      <c r="B215" s="12"/>
+      <c r="C215" s="12"/>
+      <c r="D215" s="12"/>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A217" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B217" s="5" t="s">
+      <c r="A217" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B217" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C217" s="5" t="s">
+      <c r="C217" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D217" s="4" t="s">
+      <c r="D217" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D218" s="3">
+      <c r="D218" s="11">
         <f>C218-B218</f>
         <v>0</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D219" s="3">
+      <c r="D219" s="11">
         <f>C219-B219</f>
         <v>0</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D220" s="3">
+      <c r="D220" s="11">
         <f t="shared" ref="D220" si="28">C220-B220</f>
         <v>0</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A221" s="6"/>
-      <c r="D221" s="3">
+      <c r="A221" s="4"/>
+      <c r="D221" s="11">
         <f>C221-B221</f>
         <v>0</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D222" s="3">
+      <c r="D222" s="11">
         <f>C222-B222</f>
         <v>0</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D223" s="3">
+      <c r="D223" s="11">
         <f>C223-B223</f>
         <v>0</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D224" s="3">
+      <c r="D224" s="11">
         <f>C224-B224</f>
         <v>0</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D225" s="3">
+      <c r="D225" s="11">
         <f t="shared" ref="D225" si="29">C225-B225</f>
         <v>0</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D226" s="3">
+      <c r="D226" s="11">
         <f>C226-B226</f>
         <v>0</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D227" s="3">
+      <c r="D227" s="11">
         <f t="shared" ref="D227:D229" si="30">C227-B227</f>
         <v>0</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D228" s="3">
+      <c r="D228" s="11">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D229" s="3">
+      <c r="D229" s="11">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C230" s="2" t="s">
+      <c r="C230" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D230" s="3">
+      <c r="D230" s="11">
         <f>SUM(D218:D229)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A232" s="9" t="s">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A232" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B232" s="9"/>
-      <c r="C232" s="9"/>
-      <c r="D232" s="9"/>
+      <c r="B232" s="12"/>
+      <c r="C232" s="12"/>
+      <c r="D232" s="12"/>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A234" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B234" s="5" t="s">
+      <c r="A234" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B234" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C234" s="5" t="s">
+      <c r="C234" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D234" s="4" t="s">
+      <c r="D234" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A235" t="s">
+      <c r="A235" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B235" s="2">
+      <c r="B235" s="10">
         <v>0.45833333333333331</v>
       </c>
-      <c r="C235" s="2">
+      <c r="C235" s="10">
         <v>0.47916666666666669</v>
       </c>
-      <c r="D235" s="3">
+      <c r="D235" s="11">
         <f>C235-B235</f>
         <v>2.083333333333337E-2</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A236" t="s">
+      <c r="A236" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B236" s="2">
+      <c r="B236" s="10">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C236" s="2">
+      <c r="C236" s="10">
         <v>0.14583333333333334</v>
       </c>
-      <c r="D236" s="3">
+      <c r="D236" s="11">
         <f>C236-B236</f>
         <v>6.2500000000000014E-2</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A237" t="s">
+      <c r="A237" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B237" s="2">
+      <c r="B237" s="10">
         <v>0.6875</v>
       </c>
-      <c r="C237" s="2">
+      <c r="C237" s="10">
         <v>0.8125</v>
       </c>
-      <c r="D237" s="3">
+      <c r="D237" s="11">
         <f t="shared" ref="D237" si="31">C237-B237</f>
         <v>0.125</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A238" s="6" t="s">
+      <c r="A238" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B238" s="2">
+      <c r="B238" s="10">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="C238" s="2">
+      <c r="C238" s="10">
         <v>0.14583333333333334</v>
       </c>
-      <c r="D238" s="3">
+      <c r="D238" s="11">
         <f>C238-B238</f>
         <v>0.10416666666666669</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A239" t="s">
+      <c r="A239" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B239" s="2">
+      <c r="B239" s="10">
         <v>0.5</v>
       </c>
-      <c r="C239" s="2">
+      <c r="C239" s="10">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D239" s="3">
+      <c r="D239" s="11">
         <f>C239-B239</f>
         <v>4.166666666666663E-2</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A240" t="s">
+      <c r="A240" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B240" s="2">
+      <c r="B240" s="10">
         <v>0.46180555555555558</v>
       </c>
-      <c r="C240" s="2">
+      <c r="C240" s="10">
         <v>0.47222222222222227</v>
       </c>
-      <c r="D240" s="3">
+      <c r="D240" s="11">
         <f>C240-B240</f>
         <v>1.0416666666666685E-2</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A241" t="s">
+      <c r="A241" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B241" s="2">
+      <c r="B241" s="10">
         <v>0.38541666666666669</v>
       </c>
-      <c r="C241" s="2">
+      <c r="C241" s="10">
         <v>0.42708333333333331</v>
       </c>
-      <c r="D241" s="3">
+      <c r="D241" s="11">
         <f>C241-B241</f>
         <v>4.166666666666663E-2</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A242" t="s">
+      <c r="A242" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B242" s="2">
+      <c r="B242" s="10">
         <v>0.54166666666666663</v>
       </c>
-      <c r="C242" s="2">
+      <c r="C242" s="10">
         <v>0.56597222222222221</v>
       </c>
-      <c r="D242" s="3">
+      <c r="D242" s="11">
         <f t="shared" ref="D242" si="32">C242-B242</f>
         <v>2.430555555555558E-2</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D243" s="3">
+      <c r="D243" s="11">
         <f>C243-B243</f>
         <v>0</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D244" s="3">
+      <c r="D244" s="11">
         <f t="shared" ref="D244:D246" si="33">C244-B244</f>
         <v>0</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D245" s="3">
+      <c r="D245" s="11">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D246" s="3">
+      <c r="D246" s="11">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C247" s="2" t="s">
+      <c r="C247" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D247" s="3">
+      <c r="D247" s="11">
         <f>SUM(D235:D246)</f>
         <v>0.43055555555555558</v>
       </c>
     </row>
-    <row r="249" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A249" s="9" t="s">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A249" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B249" s="9"/>
-      <c r="C249" s="9"/>
-      <c r="D249" s="9"/>
+      <c r="B249" s="12"/>
+      <c r="C249" s="12"/>
+      <c r="D249" s="12"/>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A251" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B251" s="5" t="s">
+      <c r="A251" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B251" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C251" s="5" t="s">
+      <c r="C251" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D251" s="4" t="s">
+      <c r="D251" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A252" t="s">
+      <c r="A252" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B252" s="2">
+      <c r="B252" s="10">
         <v>0.875</v>
       </c>
-      <c r="C252" s="2">
+      <c r="C252" s="10">
         <v>0.89583333333333337</v>
       </c>
-      <c r="D252" s="3">
+      <c r="D252" s="11">
         <f>C252-B252</f>
         <v>2.083333333333337E-2</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A253" t="s">
+      <c r="A253" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B253" s="2">
+      <c r="B253" s="10">
         <v>0.91666666666666663</v>
       </c>
-      <c r="C253" s="2">
+      <c r="C253" s="10">
         <v>0.95833333333333337</v>
       </c>
-      <c r="D253" s="3">
+      <c r="D253" s="11">
         <f>C253-B253</f>
         <v>4.1666666666666741E-2</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A254" t="s">
+      <c r="A254" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="B254" s="2">
+      <c r="B254" s="10">
         <v>0.61458333333333337</v>
       </c>
-      <c r="C254" s="2">
+      <c r="C254" s="10">
         <v>0.6875</v>
       </c>
-      <c r="D254" s="3">
+      <c r="D254" s="11">
         <f t="shared" ref="D254" si="34">C254-B254</f>
         <v>7.291666666666663E-2</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A255" s="6" t="s">
+      <c r="A255" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B255" s="2">
+      <c r="B255" s="10">
         <v>0.59375</v>
       </c>
-      <c r="C255" s="2">
+      <c r="C255" s="10">
         <v>0.625</v>
       </c>
-      <c r="D255" s="3">
+      <c r="D255" s="11">
         <f>C255-B255</f>
         <v>3.125E-2</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D256" s="3">
+      <c r="D256" s="11">
         <f>C256-B256</f>
         <v>0</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D257" s="3">
+      <c r="D257" s="11">
         <f>C257-B257</f>
         <v>0</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D258" s="3">
+      <c r="D258" s="11">
         <f>C258-B258</f>
         <v>0</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D259" s="3">
+      <c r="D259" s="11">
         <f t="shared" ref="D259" si="35">C259-B259</f>
         <v>0</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D260" s="3">
+      <c r="D260" s="11">
         <f>C260-B260</f>
         <v>0</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D261" s="3">
+      <c r="D261" s="11">
         <f t="shared" ref="D261:D263" si="36">C261-B261</f>
         <v>0</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D262" s="3">
+      <c r="D262" s="11">
         <f t="shared" si="36"/>
         <v>0</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D263" s="3">
+      <c r="D263" s="11">
         <f t="shared" si="36"/>
         <v>0</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C264" s="2" t="s">
+      <c r="C264" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D264" s="3">
+      <c r="D264" s="11">
         <f>SUM(D252:D263)</f>
         <v>0.16666666666666674</v>
       </c>
     </row>
-    <row r="266" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A266" s="9" t="s">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A266" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B266" s="9"/>
-      <c r="C266" s="9"/>
-      <c r="D266" s="9"/>
+      <c r="B266" s="12"/>
+      <c r="C266" s="12"/>
+      <c r="D266" s="12"/>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A268" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B268" s="5" t="s">
+      <c r="A268" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B268" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C268" s="5" t="s">
+      <c r="C268" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D268" s="4" t="s">
+      <c r="D268" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3143,14 +3167,14 @@
       <c r="A269" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B269" s="8">
+      <c r="B269" s="6">
         <v>0.60416666666666663</v>
       </c>
-      <c r="C269" s="8">
+      <c r="C269" s="6">
         <v>0.6875</v>
       </c>
-      <c r="D269" s="7">
-        <f t="shared" ref="D269:D277" si="37">C269-B269</f>
+      <c r="D269" s="5">
+        <f t="shared" ref="D269:D280" si="37">C269-B269</f>
         <v>8.333333333333337E-2</v>
       </c>
     </row>
@@ -3158,13 +3182,13 @@
       <c r="A270" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B270" s="8">
+      <c r="B270" s="6">
         <v>6.9444444444444447E-4</v>
       </c>
-      <c r="C270" s="8">
+      <c r="C270" s="6">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D270" s="7">
+      <c r="D270" s="5">
         <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
@@ -3173,13 +3197,13 @@
       <c r="A271" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B271" s="8">
+      <c r="B271" s="6">
         <v>0.57291666666666663</v>
       </c>
-      <c r="C271" s="8">
+      <c r="C271" s="6">
         <v>0.60416666666666663</v>
       </c>
-      <c r="D271" s="7">
+      <c r="D271" s="5">
         <f t="shared" si="37"/>
         <v>3.125E-2</v>
       </c>
@@ -3188,13 +3212,13 @@
       <c r="A272" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B272" s="8">
+      <c r="B272" s="6">
         <v>6.9444444444444447E-4</v>
       </c>
-      <c r="C272" s="8">
+      <c r="C272" s="6">
         <v>2.8472222222222222E-2</v>
       </c>
-      <c r="D272" s="7">
+      <c r="D272" s="5">
         <f t="shared" si="37"/>
         <v>2.7777777777777776E-2</v>
       </c>
@@ -3203,13 +3227,13 @@
       <c r="A273" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B273" s="8">
+      <c r="B273" s="6">
         <v>0.52777777777777779</v>
       </c>
-      <c r="C273" s="8">
+      <c r="C273" s="6">
         <v>0.60416666666666663</v>
       </c>
-      <c r="D273" s="7">
+      <c r="D273" s="5">
         <f t="shared" si="37"/>
         <v>7.638888888888884E-2</v>
       </c>
@@ -3218,13 +3242,13 @@
       <c r="A274" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B274" s="8">
+      <c r="B274" s="6">
         <v>6.25E-2</v>
       </c>
-      <c r="C274" s="8">
+      <c r="C274" s="6">
         <v>9.7222222222222224E-2</v>
       </c>
-      <c r="D274" s="7">
+      <c r="D274" s="5">
         <f t="shared" si="37"/>
         <v>3.4722222222222224E-2</v>
       </c>
@@ -3233,13 +3257,13 @@
       <c r="A275" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B275" s="8">
+      <c r="B275" s="6">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C275" s="8">
+      <c r="C275" s="6">
         <v>0.46180555555555558</v>
       </c>
-      <c r="D275" s="7">
+      <c r="D275" s="5">
         <f t="shared" si="37"/>
         <v>4.5138888888888895E-2</v>
       </c>
@@ -3248,36 +3272,252 @@
       <c r="A276" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B276" s="8">
+      <c r="B276" s="6">
         <v>0.53472222222222221</v>
       </c>
-      <c r="C276" s="8">
+      <c r="C276" s="6">
         <v>0.61111111111111105</v>
       </c>
-      <c r="D276" s="7">
+      <c r="D276" s="5">
         <f t="shared" si="37"/>
         <v>7.638888888888884E-2</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A277" s="1"/>
-      <c r="B277" s="8"/>
-      <c r="D277" s="7">
+      <c r="A277" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B277" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C277" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="D277" s="5">
         <f t="shared" si="37"/>
-        <v>0</v>
-      </c>
+        <v>4.166666666666663E-2</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A278" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B278" s="6">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="C278" s="6">
+        <v>0.90625</v>
+      </c>
+      <c r="D278" s="5">
+        <f t="shared" si="37"/>
+        <v>5.208333333333337E-2</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A279" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B279" s="6">
+        <v>0.4375</v>
+      </c>
+      <c r="C279" s="6">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D279" s="5">
+        <f t="shared" si="37"/>
+        <v>2.0833333333333315E-2</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A280" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B280" s="6">
+        <v>0.59375</v>
+      </c>
+      <c r="C280" s="6">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="D280" s="5">
+        <f t="shared" si="37"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A281" s="1"/>
+      <c r="B281" s="6"/>
+      <c r="C281" s="6"/>
+      <c r="D281" s="1"/>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C282" s="8" t="s">
+      <c r="A282" s="1"/>
+      <c r="B282" s="6"/>
+      <c r="C282" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D282" s="7">
+      <c r="D282" s="5">
         <f>SUM(D269:D281)</f>
-        <v>0.41666666666666657</v>
+        <v>0.55208333333333315</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A286" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B286" s="12"/>
+      <c r="C286" s="12"/>
+      <c r="D286" s="12"/>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A288" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B288" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C288" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D288" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A289" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B289" s="6">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C289" s="6">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="D289" s="5">
+        <f t="shared" ref="D289:D300" si="38">C289-B289</f>
+        <v>0.14583333333333326</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A290" s="1"/>
+      <c r="B290" s="6"/>
+      <c r="C290" s="6"/>
+      <c r="D290" s="5">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A291" s="1"/>
+      <c r="B291" s="6"/>
+      <c r="C291" s="6"/>
+      <c r="D291" s="5">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A292" s="1"/>
+      <c r="B292" s="6"/>
+      <c r="C292" s="6"/>
+      <c r="D292" s="5">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A293" s="1"/>
+      <c r="B293" s="6"/>
+      <c r="C293" s="6"/>
+      <c r="D293" s="5">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A294" s="1"/>
+      <c r="B294" s="6"/>
+      <c r="C294" s="6"/>
+      <c r="D294" s="5">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A295" s="1"/>
+      <c r="B295" s="6"/>
+      <c r="C295" s="6"/>
+      <c r="D295" s="5">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A296" s="1"/>
+      <c r="B296" s="6"/>
+      <c r="C296" s="6"/>
+      <c r="D296" s="5">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A297" s="1"/>
+      <c r="B297" s="6"/>
+      <c r="C297" s="6"/>
+      <c r="D297" s="5">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A298" s="1"/>
+      <c r="B298" s="6"/>
+      <c r="C298" s="6"/>
+      <c r="D298" s="5">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A299" s="1"/>
+      <c r="B299" s="6"/>
+      <c r="C299" s="6"/>
+      <c r="D299" s="5">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A300" s="1"/>
+      <c r="B300" s="6"/>
+      <c r="C300" s="6"/>
+      <c r="D300" s="5">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A301" s="1"/>
+      <c r="B301" s="6"/>
+      <c r="C301" s="6"/>
+      <c r="D301" s="1"/>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A302" s="1"/>
+      <c r="B302" s="6"/>
+      <c r="C302" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D302" s="5">
+        <f>SUM(D289:D301)</f>
+        <v>0.14583333333333326</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
+    <mergeCell ref="A127:D127"/>
+    <mergeCell ref="A110:D110"/>
+    <mergeCell ref="A286:D286"/>
     <mergeCell ref="A266:D266"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A20:D20"/>
@@ -3292,8 +3532,6 @@
     <mergeCell ref="A162:D162"/>
     <mergeCell ref="A180:D180"/>
     <mergeCell ref="A145:D145"/>
-    <mergeCell ref="A127:D127"/>
-    <mergeCell ref="A110:D110"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
after fixing firm fixed effects. before changing variable names
</commit_message>
<xml_diff>
--- a/Administrative-Noam/LoggedHours.xlsx
+++ b/Administrative-Noam/LoggedHours.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="115">
   <si>
     <t>Date</t>
   </si>
@@ -336,6 +336,42 @@
   </si>
   <si>
     <t>Thursday, Feb 1, 2018</t>
+  </si>
+  <si>
+    <t>Friday, Feb 2, 2018</t>
+  </si>
+  <si>
+    <t>Thursday, Feb 8, 2018</t>
+  </si>
+  <si>
+    <t>really Wednesday 1/31</t>
+  </si>
+  <si>
+    <t>really Thursday 2/1</t>
+  </si>
+  <si>
+    <t>really Friday 2/2</t>
+  </si>
+  <si>
+    <t>really Saturday 2/3</t>
+  </si>
+  <si>
+    <t>Friday, Feb 9, 2018</t>
+  </si>
+  <si>
+    <t>really Sunday 2/4</t>
+  </si>
+  <si>
+    <t>really Thursday 2/8</t>
+  </si>
+  <si>
+    <t>Saturday, Feb 10, 2018</t>
+  </si>
+  <si>
+    <t>Sunday, Feb 11, 2018</t>
+  </si>
+  <si>
+    <t>really Friday 2/9</t>
   </si>
 </sst>
 </file>
@@ -757,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E302"/>
+  <dimension ref="A1:F302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A282" zoomScale="98" workbookViewId="0">
-      <selection activeCell="D289" sqref="D289"/>
+    <sheetView tabSelected="1" topLeftCell="A285" zoomScale="98" workbookViewId="0">
+      <selection activeCell="D297" sqref="D297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -768,7 +804,9 @@
     <col min="1" max="1" width="22.83203125" style="9" customWidth="1"/>
     <col min="2" max="3" width="10.83203125" style="10"/>
     <col min="4" max="4" width="12.33203125" style="9" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="9"/>
+    <col min="5" max="5" width="10.83203125" style="9"/>
+    <col min="6" max="6" width="21.83203125" style="9" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -3382,7 +3420,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A289" s="1" t="s">
         <v>102</v>
       </c>
@@ -3396,44 +3434,80 @@
         <f t="shared" ref="D289:D300" si="38">C289-B289</f>
         <v>0.14583333333333326</v>
       </c>
-    </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A290" s="1"/>
-      <c r="B290" s="6"/>
-      <c r="C290" s="6"/>
+      <c r="F289" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A290" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B290" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C290" s="6">
+        <v>0.61458333333333337</v>
+      </c>
       <c r="D290" s="5">
         <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A291" s="1"/>
-      <c r="B291" s="6"/>
-      <c r="C291" s="6"/>
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A291" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B291" s="6">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C291" s="6">
+        <v>0.98958333333333337</v>
+      </c>
       <c r="D291" s="5">
         <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A292" s="1"/>
-      <c r="B292" s="6"/>
-      <c r="C292" s="6"/>
+        <v>0.15625</v>
+      </c>
+      <c r="F291" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A292" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B292" s="6">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C292" s="6">
+        <v>0.76041666666666663</v>
+      </c>
       <c r="D292" s="5">
         <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A293" s="1"/>
-      <c r="B293" s="6"/>
-      <c r="C293" s="6"/>
+        <v>5.2083333333333259E-2</v>
+      </c>
+      <c r="F292" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A293" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B293" s="6">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="C293" s="6">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="D293" s="5">
         <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.2">
+        <v>9.375E-2</v>
+      </c>
+      <c r="F293" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A294" s="1"/>
       <c r="B294" s="6"/>
       <c r="C294" s="6"/>
@@ -3441,35 +3515,65 @@
         <f t="shared" si="38"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A295" s="1"/>
-      <c r="B295" s="6"/>
-      <c r="C295" s="6"/>
+      <c r="F294" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A295" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B295" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="C295" s="6">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="D295" s="5">
         <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A296" s="1"/>
-      <c r="B296" s="6"/>
-      <c r="C296" s="6"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F295" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A296" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B296" s="6">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C296" s="6">
+        <v>0.95833333333333337</v>
+      </c>
       <c r="D296" s="5">
         <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A297" s="1"/>
-      <c r="B297" s="6"/>
-      <c r="C297" s="6"/>
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="F296" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A297" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B297" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C297" s="6">
+        <v>0.6875</v>
+      </c>
       <c r="D297" s="5">
         <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.10416666666666663</v>
+      </c>
+      <c r="F297" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A298" s="1"/>
       <c r="B298" s="6"/>
       <c r="C298" s="6"/>
@@ -3478,7 +3582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A299" s="1"/>
       <c r="B299" s="6"/>
       <c r="C299" s="6"/>
@@ -3487,7 +3591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A300" s="1"/>
       <c r="B300" s="6"/>
       <c r="C300" s="6"/>
@@ -3496,13 +3600,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A301" s="1"/>
       <c r="B301" s="6"/>
       <c r="C301" s="6"/>
       <c r="D301" s="1"/>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A302" s="1"/>
       <c r="B302" s="6"/>
       <c r="C302" s="6" t="s">
@@ -3510,7 +3614,7 @@
       </c>
       <c r="D302" s="5">
         <f>SUM(D289:D301)</f>
-        <v>0.14583333333333326</v>
+        <v>0.64583333333333326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>